<commit_message>
diagonal_5x5 environment added toy groups
</commit_message>
<xml_diff>
--- a/environments/diagonal_5x5/Grid Representation.xlsx
+++ b/environments/diagonal_5x5/Grid Representation.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimichai/projects/phd/fair-network-expansion/environments/diagonal_5x5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C295B2A-C0E9-224B-8BB9-38D7375325C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F9DBDB-9719-4E4C-9BCE-FDDCD525DF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{119A3763-3FAF-8D43-924D-B490D1D6BAA1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Groups" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,6 +34,14 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>OD</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -45,15 +53,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -61,12 +75,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,37 +412,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B68749-DF5B-5546-B836-5CADB7D7041F}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D2">
-        <v>3</v>
-      </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <f>C8/MAX(C$8:C$15)</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:D15" si="0">C9/MAX(C$8:C$15)</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>10</v>
+      <c r="C14" s="2">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="2">
+        <f>SUM(C8:C15)</f>
+        <v>74</v>
+      </c>
+      <c r="D17">
+        <f>SUM(D8:D15)</f>
+        <v>6.1666666666666661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extra od experiments for diagonal_5x5
</commit_message>
<xml_diff>
--- a/environments/diagonal_5x5/Grid Representation.xlsx
+++ b/environments/diagonal_5x5/Grid Representation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimichai/projects/phd/fair-network-expansion/environments/diagonal_5x5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F9DBDB-9719-4E4C-9BCE-FDDCD525DF6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F049AF3-1254-AF4A-A9EE-57F41D1A228C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{119A3763-3FAF-8D43-924D-B490D1D6BAA1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16140" xr2:uid="{119A3763-3FAF-8D43-924D-B490D1D6BAA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -63,6 +63,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -94,10 +100,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +422,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +489,7 @@
       <c r="C8" s="2">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <f>C8/MAX(C$8:C$15)</f>
         <v>0.83333333333333337</v>
       </c>
@@ -497,7 +504,7 @@
       <c r="C9" s="2">
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <f t="shared" ref="D9:D15" si="0">C9/MAX(C$8:C$15)</f>
         <v>0.83333333333333337</v>
       </c>
@@ -512,7 +519,7 @@
       <c r="C10" s="2">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
@@ -527,7 +534,7 @@
       <c r="C11" s="2">
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>

</xml_diff>